<commit_message>
modifier les algo de génération des contrats et bilans pour que ils travaillent seulement avec des redoublements, pas tous les étudiants
</commit_message>
<xml_diff>
--- a/Liste+Bilan contrat/EnteteJury.xlsx
+++ b/Liste+Bilan contrat/EnteteJury.xlsx
@@ -115,384 +115,387 @@
     <t xml:space="preserve">E001</t>
   </si>
   <si>
+    <t xml:space="preserve">Bernard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Camille</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chevalier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E003</t>
+  </si>
+  <si>
     <t xml:space="preserve">Vincent</t>
   </si>
   <si>
+    <t xml:space="preserve">Louis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Durand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hugo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lucas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Garnier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fournier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inès</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zoé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nathan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moulin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Morin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Louise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jules</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fontaine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Noah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thomas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Léa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Martin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moreau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bertrand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leroy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Garcia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raphaël</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E028</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E029</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Robert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E030</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Michel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E031</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E032</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E033</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E034</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sarah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E035</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E036</t>
+  </si>
+  <si>
+    <t xml:space="preserve">David</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E037</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E038</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E039</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laurent</t>
+  </si>
+  <si>
     <t xml:space="preserve">Arthur</t>
   </si>
   <si>
-    <t xml:space="preserve">E002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Simon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paul</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Moulin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Camille</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fournier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Leroy</t>
+    <t xml:space="preserve">E040</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E041</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Petit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E042</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sacha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E043</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E044</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E045</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E046</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E047</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E048</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E049</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E050</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E051</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dubois</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E052</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Léo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E053</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E054</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gabriel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E055</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E056</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E057</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E058</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E059</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E060</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Richard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E061</t>
   </si>
   <si>
     <t xml:space="preserve">Lina</t>
   </si>
   <si>
-    <t xml:space="preserve">E006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Michel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Emma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E007</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Roux</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jules</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Morin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Louis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Durand</t>
+    <t xml:space="preserve">E062</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E063</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E064</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E065</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E066</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E067</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E068</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E069</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E070</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E071</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E072</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E073</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E074</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E075</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E076</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E077</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E078</t>
   </si>
   <si>
     <t xml:space="preserve">Chloé</t>
   </si>
   <si>
-    <t xml:space="preserve">E010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Roger</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Raphaël</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Noah</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fontaine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Robert</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zoé</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thomas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Léo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hugo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Léa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Richard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sarah</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Moreau</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bertrand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Martin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jade</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gabriel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lucas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E027</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bernard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Louise</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E028</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E029</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E030</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E031</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E032</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E033</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E034</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E035</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E036</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E037</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inès</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E038</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chevalier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nathan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E039</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E040</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E041</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E042</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E043</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E044</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E045</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E046</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E047</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E048</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E049</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Garnier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E050</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E051</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Petit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E052</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E053</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E054</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sacha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E055</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E056</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E057</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E058</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E059</t>
-  </si>
-  <si>
-    <t xml:space="preserve">David</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E060</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E061</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E062</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E063</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E064</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E065</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E066</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Laurent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E067</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E068</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E069</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E070</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E071</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E072</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E073</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E074</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dubois</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E075</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E076</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E077</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E078</t>
-  </si>
-  <si>
     <t xml:space="preserve">E079</t>
   </si>
   <si>
@@ -500,9 +503,6 @@
   </si>
   <si>
     <t xml:space="preserve">E081</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Garcia</t>
   </si>
   <si>
     <t xml:space="preserve">E082</t>
@@ -1024,7 +1024,7 @@
         <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="R3" t="s">
         <v>181</v>
@@ -1032,13 +1032,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" t="s">
         <v>37</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>38</v>
-      </c>
-      <c r="C4" t="s">
-        <v>39</v>
       </c>
       <c r="R4" t="s">
         <v>181</v>
@@ -1046,13 +1046,13 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" t="s">
         <v>40</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>41</v>
-      </c>
-      <c r="C5" t="s">
-        <v>36</v>
       </c>
       <c r="R5" t="s">
         <v>182</v>
@@ -1063,10 +1063,10 @@
         <v>42</v>
       </c>
       <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
         <v>43</v>
-      </c>
-      <c r="C6" t="s">
-        <v>44</v>
       </c>
       <c r="R6" t="s">
         <v>181</v>
@@ -1074,13 +1074,13 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" t="s">
         <v>45</v>
       </c>
-      <c r="B7" t="s">
-        <v>46</v>
-      </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="R7" t="s">
         <v>182</v>
@@ -1088,13 +1088,13 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" t="s">
         <v>48</v>
-      </c>
-      <c r="B8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" t="s">
-        <v>50</v>
       </c>
       <c r="R8" t="s">
         <v>182</v>
@@ -1102,13 +1102,13 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="R9" t="s">
         <v>182</v>
@@ -1116,13 +1116,13 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="R10" t="s">
         <v>181</v>
@@ -1130,13 +1130,13 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B11" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="R11" t="s">
         <v>183</v>
@@ -1144,13 +1144,13 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="C12" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="R12" t="s">
         <v>182</v>
@@ -1158,13 +1158,13 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B13" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="R13" t="s">
         <v>182</v>
@@ -1172,13 +1172,13 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B14" t="s">
-        <v>65</v>
+        <v>35</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="R14" t="s">
         <v>183</v>
@@ -1186,13 +1186,13 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B15" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="R15" t="s">
         <v>182</v>
@@ -1200,13 +1200,13 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B16" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="R16" t="s">
         <v>181</v>
@@ -1214,13 +1214,13 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="C17" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="R17" t="s">
         <v>183</v>
@@ -1228,13 +1228,13 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B18" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C18" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="R18" t="s">
         <v>181</v>
@@ -1242,13 +1242,13 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="C19" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="R19" t="s">
         <v>181</v>
@@ -1256,13 +1256,13 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B20" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C20" t="s">
-        <v>78</v>
+        <v>33</v>
       </c>
       <c r="R20" t="s">
         <v>183</v>
@@ -1270,13 +1270,13 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="C21" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="R21" t="s">
         <v>183</v>
@@ -1284,13 +1284,13 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B22" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C22" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="R22" t="s">
         <v>183</v>
@@ -1298,13 +1298,13 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B23" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C23" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="R23" t="s">
         <v>183</v>
@@ -1312,13 +1312,13 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B24" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C24" t="s">
-        <v>87</v>
+        <v>61</v>
       </c>
       <c r="R24" t="s">
         <v>181</v>
@@ -1326,13 +1326,13 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B25" t="s">
-        <v>35</v>
+        <v>83</v>
       </c>
       <c r="C25" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="R25" t="s">
         <v>182</v>
@@ -1340,13 +1340,13 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B26" t="s">
-        <v>43</v>
+        <v>86</v>
       </c>
       <c r="C26" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="R26" t="s">
         <v>181</v>
@@ -1354,13 +1354,13 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B27" t="s">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="C27" t="s">
-        <v>92</v>
+        <v>41</v>
       </c>
       <c r="R27" t="s">
         <v>182</v>
@@ -1368,13 +1368,13 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B28" t="s">
-        <v>94</v>
+        <v>40</v>
       </c>
       <c r="C28" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="R28" t="s">
         <v>183</v>
@@ -1382,13 +1382,13 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B29" t="s">
-        <v>65</v>
+        <v>86</v>
       </c>
       <c r="C29" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="R29" t="s">
         <v>182</v>
@@ -1396,13 +1396,13 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B30" t="s">
-        <v>35</v>
+        <v>94</v>
       </c>
       <c r="C30" t="s">
-        <v>78</v>
+        <v>33</v>
       </c>
       <c r="R30" t="s">
         <v>181</v>
@@ -1410,13 +1410,13 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B31" t="s">
-        <v>38</v>
+        <v>96</v>
       </c>
       <c r="C31" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="R31" t="s">
         <v>182</v>
@@ -1424,13 +1424,13 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
       <c r="C32" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="R32" t="s">
         <v>183</v>
@@ -1438,13 +1438,13 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B33" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C33" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="R33" t="s">
         <v>181</v>
@@ -1452,13 +1452,13 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B34" t="s">
-        <v>35</v>
+        <v>100</v>
       </c>
       <c r="C34" t="s">
-        <v>78</v>
+        <v>52</v>
       </c>
       <c r="R34" t="s">
         <v>181</v>
@@ -1466,13 +1466,13 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B35" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="C35" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="R35" t="s">
         <v>183</v>
@@ -1480,13 +1480,13 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B36" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="C36" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="R36" t="s">
         <v>181</v>
@@ -1494,13 +1494,13 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
+        <v>104</v>
+      </c>
+      <c r="B37" t="s">
         <v>105</v>
       </c>
-      <c r="B37" t="s">
-        <v>84</v>
-      </c>
       <c r="C37" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="R37" t="s">
         <v>182</v>
@@ -1511,10 +1511,10 @@
         <v>106</v>
       </c>
       <c r="B38" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="C38" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="R38" t="s">
         <v>183</v>
@@ -1522,13 +1522,13 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B39" t="s">
-        <v>109</v>
+        <v>83</v>
       </c>
       <c r="C39" t="s">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="R39" t="s">
         <v>181</v>
@@ -1536,10 +1536,10 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B40" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="C40" t="s">
         <v>110</v>
@@ -1550,13 +1550,13 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B41" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="C41" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="R41" t="s">
         <v>183</v>
@@ -1564,13 +1564,13 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
+        <v>112</v>
+      </c>
+      <c r="B42" t="s">
         <v>113</v>
       </c>
-      <c r="B42" t="s">
-        <v>82</v>
-      </c>
       <c r="C42" t="s">
-        <v>67</v>
+        <v>110</v>
       </c>
       <c r="R42" t="s">
         <v>182</v>
@@ -1581,10 +1581,10 @@
         <v>114</v>
       </c>
       <c r="B43" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="C43" t="s">
-        <v>59</v>
+        <v>115</v>
       </c>
       <c r="R43" t="s">
         <v>181</v>
@@ -1592,10 +1592,10 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B44" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C44" t="s">
         <v>61</v>
@@ -1606,13 +1606,13 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B45" t="s">
-        <v>35</v>
+        <v>96</v>
       </c>
       <c r="C45" t="s">
-        <v>110</v>
+        <v>65</v>
       </c>
       <c r="R45" t="s">
         <v>183</v>
@@ -1620,13 +1620,13 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B46" t="s">
-        <v>41</v>
+        <v>73</v>
       </c>
       <c r="C46" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="R46" t="s">
         <v>181</v>
@@ -1634,13 +1634,13 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B47" t="s">
-        <v>63</v>
+        <v>100</v>
       </c>
       <c r="C47" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="R47" t="s">
         <v>183</v>
@@ -1648,13 +1648,13 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B48" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C48" t="s">
-        <v>53</v>
+        <v>87</v>
       </c>
       <c r="R48" t="s">
         <v>181</v>
@@ -1662,13 +1662,13 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B49" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C49" t="s">
-        <v>121</v>
+        <v>54</v>
       </c>
       <c r="R49" t="s">
         <v>182</v>
@@ -1679,10 +1679,10 @@
         <v>122</v>
       </c>
       <c r="B50" t="s">
-        <v>123</v>
+        <v>77</v>
       </c>
       <c r="C50" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="R50" t="s">
         <v>183</v>
@@ -1690,13 +1690,13 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B51" t="s">
-        <v>82</v>
+        <v>37</v>
       </c>
       <c r="C51" t="s">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="R51" t="s">
         <v>182</v>
@@ -1704,13 +1704,13 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
+        <v>124</v>
+      </c>
+      <c r="B52" t="s">
         <v>125</v>
       </c>
-      <c r="B52" t="s">
-        <v>126</v>
-      </c>
       <c r="C52" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="R52" t="s">
         <v>183</v>
@@ -1718,13 +1718,13 @@
     </row>
     <row r="53">
       <c r="A53" t="s">
+        <v>126</v>
+      </c>
+      <c r="B53" t="s">
+        <v>125</v>
+      </c>
+      <c r="C53" t="s">
         <v>127</v>
-      </c>
-      <c r="B53" t="s">
-        <v>35</v>
-      </c>
-      <c r="C53" t="s">
-        <v>90</v>
       </c>
       <c r="R53" t="s">
         <v>183</v>
@@ -1735,10 +1735,10 @@
         <v>128</v>
       </c>
       <c r="B54" t="s">
-        <v>38</v>
+        <v>105</v>
       </c>
       <c r="C54" t="s">
-        <v>47</v>
+        <v>110</v>
       </c>
       <c r="R54" t="s">
         <v>181</v>
@@ -1749,7 +1749,7 @@
         <v>129</v>
       </c>
       <c r="B55" t="s">
-        <v>38</v>
+        <v>109</v>
       </c>
       <c r="C55" t="s">
         <v>130</v>
@@ -1763,10 +1763,10 @@
         <v>131</v>
       </c>
       <c r="B56" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="C56" t="s">
-        <v>107</v>
+        <v>127</v>
       </c>
       <c r="R56" t="s">
         <v>182</v>
@@ -1777,10 +1777,10 @@
         <v>132</v>
       </c>
       <c r="B57" t="s">
-        <v>69</v>
+        <v>105</v>
       </c>
       <c r="C57" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="R57" t="s">
         <v>183</v>
@@ -1788,13 +1788,13 @@
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B58" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="C58" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="R58" t="s">
         <v>183</v>
@@ -1802,13 +1802,13 @@
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B59" t="s">
-        <v>77</v>
+        <v>35</v>
       </c>
       <c r="C59" t="s">
-        <v>90</v>
+        <v>48</v>
       </c>
       <c r="R59" t="s">
         <v>181</v>
@@ -1816,13 +1816,13 @@
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B60" t="s">
-        <v>136</v>
+        <v>32</v>
       </c>
       <c r="C60" t="s">
-        <v>44</v>
+        <v>110</v>
       </c>
       <c r="R60" t="s">
         <v>183</v>
@@ -1833,10 +1833,10 @@
         <v>137</v>
       </c>
       <c r="B61" t="s">
-        <v>55</v>
+        <v>138</v>
       </c>
       <c r="C61" t="s">
-        <v>110</v>
+        <v>59</v>
       </c>
       <c r="R61" t="s">
         <v>182</v>
@@ -1844,13 +1844,13 @@
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B62" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="C62" t="s">
-        <v>101</v>
+        <v>140</v>
       </c>
       <c r="R62" t="s">
         <v>183</v>
@@ -1858,13 +1858,13 @@
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B63" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C63" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="R63" t="s">
         <v>181</v>
@@ -1872,13 +1872,13 @@
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B64" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="C64" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="R64" t="s">
         <v>183</v>
@@ -1886,13 +1886,13 @@
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B65" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="C65" t="s">
-        <v>73</v>
+        <v>102</v>
       </c>
       <c r="R65" t="s">
         <v>181</v>
@@ -1900,13 +1900,13 @@
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B66" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
       <c r="C66" t="s">
-        <v>39</v>
+        <v>140</v>
       </c>
       <c r="R66" t="s">
         <v>182</v>
@@ -1914,13 +1914,13 @@
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B67" t="s">
-        <v>144</v>
+        <v>83</v>
       </c>
       <c r="C67" t="s">
-        <v>90</v>
+        <v>38</v>
       </c>
       <c r="R67" t="s">
         <v>181</v>
@@ -1928,13 +1928,13 @@
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B68" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="C68" t="s">
-        <v>61</v>
+        <v>130</v>
       </c>
       <c r="R68" t="s">
         <v>182</v>
@@ -1942,13 +1942,13 @@
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B69" t="s">
-        <v>136</v>
+        <v>113</v>
       </c>
       <c r="C69" t="s">
-        <v>75</v>
+        <v>133</v>
       </c>
       <c r="R69" t="s">
         <v>182</v>
@@ -1956,13 +1956,13 @@
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B70" t="s">
-        <v>38</v>
+        <v>100</v>
       </c>
       <c r="C70" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="R70" t="s">
         <v>181</v>
@@ -1970,13 +1970,13 @@
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B71" t="s">
-        <v>46</v>
+        <v>138</v>
       </c>
       <c r="C71" t="s">
-        <v>121</v>
+        <v>65</v>
       </c>
       <c r="R71" t="s">
         <v>182</v>
@@ -1984,13 +1984,13 @@
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B72" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="C72" t="s">
-        <v>71</v>
+        <v>41</v>
       </c>
       <c r="R72" t="s">
         <v>182</v>
@@ -1998,13 +1998,13 @@
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B73" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="C73" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="R73" t="s">
         <v>181</v>
@@ -2012,13 +2012,13 @@
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B74" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="C74" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="R74" t="s">
         <v>181</v>
@@ -2026,13 +2026,13 @@
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B75" t="s">
-        <v>153</v>
+        <v>83</v>
       </c>
       <c r="C75" t="s">
-        <v>92</v>
+        <v>43</v>
       </c>
       <c r="R75" t="s">
         <v>183</v>
@@ -2043,10 +2043,10 @@
         <v>154</v>
       </c>
       <c r="B76" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C76" t="s">
-        <v>61</v>
+        <v>130</v>
       </c>
       <c r="R76" t="s">
         <v>182</v>
@@ -2057,10 +2057,10 @@
         <v>155</v>
       </c>
       <c r="B77" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="C77" t="s">
-        <v>36</v>
+        <v>110</v>
       </c>
       <c r="R77" t="s">
         <v>182</v>
@@ -2071,10 +2071,10 @@
         <v>156</v>
       </c>
       <c r="B78" t="s">
+        <v>138</v>
+      </c>
+      <c r="C78" t="s">
         <v>41</v>
-      </c>
-      <c r="C78" t="s">
-        <v>121</v>
       </c>
       <c r="R78" t="s">
         <v>183</v>
@@ -2085,10 +2085,10 @@
         <v>157</v>
       </c>
       <c r="B79" t="s">
-        <v>32</v>
+        <v>86</v>
       </c>
       <c r="C79" t="s">
-        <v>71</v>
+        <v>158</v>
       </c>
       <c r="R79" t="s">
         <v>182</v>
@@ -2096,13 +2096,13 @@
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B80" t="s">
-        <v>41</v>
+        <v>100</v>
       </c>
       <c r="C80" t="s">
-        <v>130</v>
+        <v>102</v>
       </c>
       <c r="R80" t="s">
         <v>183</v>
@@ -2110,13 +2110,13 @@
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B81" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C81" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="R81" t="s">
         <v>183</v>
@@ -2124,13 +2124,13 @@
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B82" t="s">
-        <v>161</v>
+        <v>58</v>
       </c>
       <c r="C82" t="s">
-        <v>61</v>
+        <v>127</v>
       </c>
       <c r="R82" t="s">
         <v>182</v>
@@ -2141,10 +2141,10 @@
         <v>162</v>
       </c>
       <c r="B83" t="s">
-        <v>161</v>
+        <v>40</v>
       </c>
       <c r="C83" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="R83" t="s">
         <v>181</v>
@@ -2155,10 +2155,10 @@
         <v>163</v>
       </c>
       <c r="B84" t="s">
-        <v>35</v>
+        <v>96</v>
       </c>
       <c r="C84" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="R84" t="s">
         <v>181</v>
@@ -2169,10 +2169,10 @@
         <v>164</v>
       </c>
       <c r="B85" t="s">
+        <v>47</v>
+      </c>
+      <c r="C85" t="s">
         <v>84</v>
-      </c>
-      <c r="C85" t="s">
-        <v>87</v>
       </c>
       <c r="R85" t="s">
         <v>183</v>
@@ -2183,10 +2183,10 @@
         <v>165</v>
       </c>
       <c r="B86" t="s">
-        <v>144</v>
+        <v>100</v>
       </c>
       <c r="C86" t="s">
-        <v>53</v>
+        <v>130</v>
       </c>
       <c r="R86" t="s">
         <v>182</v>
@@ -2197,10 +2197,10 @@
         <v>166</v>
       </c>
       <c r="B87" t="s">
-        <v>153</v>
+        <v>64</v>
       </c>
       <c r="C87" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="R87" t="s">
         <v>183</v>
@@ -2211,10 +2211,10 @@
         <v>167</v>
       </c>
       <c r="B88" t="s">
-        <v>86</v>
+        <v>47</v>
       </c>
       <c r="C88" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="R88" t="s">
         <v>182</v>
@@ -2225,10 +2225,10 @@
         <v>168</v>
       </c>
       <c r="B89" t="s">
-        <v>94</v>
+        <v>37</v>
       </c>
       <c r="C89" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="R89" t="s">
         <v>183</v>
@@ -2239,10 +2239,10 @@
         <v>169</v>
       </c>
       <c r="B90" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C90" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="R90" t="s">
         <v>181</v>
@@ -2253,10 +2253,10 @@
         <v>170</v>
       </c>
       <c r="B91" t="s">
-        <v>161</v>
+        <v>37</v>
       </c>
       <c r="C91" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="R91" t="s">
         <v>181</v>
@@ -2267,10 +2267,10 @@
         <v>171</v>
       </c>
       <c r="B92" t="s">
-        <v>43</v>
+        <v>94</v>
       </c>
       <c r="C92" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="R92" t="s">
         <v>182</v>
@@ -2281,10 +2281,10 @@
         <v>172</v>
       </c>
       <c r="B93" t="s">
-        <v>84</v>
+        <v>40</v>
       </c>
       <c r="C93" t="s">
-        <v>107</v>
+        <v>67</v>
       </c>
       <c r="R93" t="s">
         <v>181</v>
@@ -2295,10 +2295,10 @@
         <v>173</v>
       </c>
       <c r="B94" t="s">
-        <v>84</v>
+        <v>45</v>
       </c>
       <c r="C94" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="R94" t="s">
         <v>183</v>
@@ -2309,10 +2309,10 @@
         <v>174</v>
       </c>
       <c r="B95" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="C95" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="R95" t="s">
         <v>182</v>
@@ -2323,10 +2323,10 @@
         <v>175</v>
       </c>
       <c r="B96" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C96" t="s">
-        <v>101</v>
+        <v>33</v>
       </c>
       <c r="R96" t="s">
         <v>182</v>
@@ -2337,10 +2337,10 @@
         <v>176</v>
       </c>
       <c r="B97" t="s">
-        <v>144</v>
+        <v>96</v>
       </c>
       <c r="C97" t="s">
-        <v>67</v>
+        <v>115</v>
       </c>
       <c r="R97" t="s">
         <v>181</v>
@@ -2351,10 +2351,10 @@
         <v>177</v>
       </c>
       <c r="B98" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="C98" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="R98" t="s">
         <v>182</v>
@@ -2365,10 +2365,10 @@
         <v>178</v>
       </c>
       <c r="B99" t="s">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="C99" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="R99" t="s">
         <v>183</v>
@@ -2379,10 +2379,10 @@
         <v>179</v>
       </c>
       <c r="B100" t="s">
-        <v>136</v>
+        <v>40</v>
       </c>
       <c r="C100" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="R100" t="s">
         <v>181</v>
@@ -2393,10 +2393,10 @@
         <v>180</v>
       </c>
       <c r="B101" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="C101" t="s">
-        <v>73</v>
+        <v>102</v>
       </c>
       <c r="R101" t="s">
         <v>181</v>

</xml_diff>